<commit_message>
Many updates to 1D FVM solver
</commit_message>
<xml_diff>
--- a/src/OscillationRates.xlsx
+++ b/src/OscillationRates.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/Documents/Research/FourierAnalysis/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02674F3E-7B10-A246-AF83-88B3628E6D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD24381-D023-8749-A2DD-EDF3B9561285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{60426555-CA7B-3641-8465-F4E60B8F88C2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{60426555-CA7B-3641-8465-F4E60B8F88C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
   <si>
     <t>kdx</t>
   </si>
@@ -184,15 +185,43 @@
   </si>
   <si>
     <t>central diff</t>
+  </si>
+  <si>
+    <t>2D FEM</t>
+  </si>
+  <si>
+    <t>1D FVM</t>
+  </si>
+  <si>
+    <t>Fourier</t>
+  </si>
+  <si>
+    <t>Decay Rates: tantheta = 0.1</t>
+  </si>
+  <si>
+    <t>Decay Rates: tantheta = 0.0</t>
+  </si>
+  <si>
+    <t>Vcol</t>
+  </si>
+  <si>
+    <t>Vcol2: hump develops for both codes around t=20</t>
+  </si>
+  <si>
+    <t>RT dominant perturbation</t>
+  </si>
+  <si>
+    <t>p and u dominate perturbation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -366,7 +395,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,13 +434,17 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -768,10 +801,10 @@
       <c r="D1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="34"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="14" t="s">
         <v>32</v>
       </c>
@@ -1523,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C084DA23-C2D9-E143-8245-CB1E8FD4B3B1}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -1555,11 +1588,11 @@
       <c r="D1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="14" t="s">
         <v>40</v>
       </c>
@@ -2261,17 +2294,17 @@
       </c>
       <c r="C39" s="1">
         <f>I39/J39*2*3.1416</f>
-        <v>0.53407199999999999</v>
-      </c>
-      <c r="H39" s="36">
-        <v>17</v>
+        <v>0.52359999999999995</v>
+      </c>
+      <c r="H39" s="34">
+        <v>5</v>
       </c>
       <c r="I39" s="1">
         <f>H39/2</f>
-        <v>8.5</v>
+        <v>2.5</v>
       </c>
       <c r="J39" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2297,4 +2330,151 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EF0E5E5-804E-294A-9445-09408EBC9CE6}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="37">
+        <v>2</v>
+      </c>
+      <c r="B3" s="38">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="C3" s="37">
+        <v>0.20966499999999999</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="37">
+        <v>2</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0.19939999999999999</v>
+      </c>
+      <c r="I3" s="37">
+        <v>0.20966499999999999</v>
+      </c>
+      <c r="J3" s="37">
+        <v>0.22932</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>67</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>48</v>
+      </c>
+      <c r="H4" s="39">
+        <v>0.50109999999999999</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0.22212699999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.49003999999999998</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>131</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5">
+        <v>168</v>
+      </c>
+      <c r="H5" s="39">
+        <v>1.01</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.91507000000000005</v>
+      </c>
+      <c r="J5">
+        <v>1.0916999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="39"/>
+      <c r="H6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="39"/>
+      <c r="H7" s="39"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="39"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>